<commit_message>
end of day 8/10/2018
</commit_message>
<xml_diff>
--- a/WR.xlsx
+++ b/WR.xlsx
@@ -1104,7 +1104,7 @@
   <dimension ref="A1:A249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,22 +1119,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>